<commit_message>
Add insertion outlines and gerber for LED panel placement
</commit_message>
<xml_diff>
--- a/PCB/LED_Panel/Assembly/BOM.xlsx
+++ b/PCB/LED_Panel/Assembly/BOM.xlsx
@@ -104,7 +104,7 @@
     <t>Click here</t>
   </si>
   <si>
-    <t>Stock: 14650</t>
+    <t>Stock: 14520</t>
   </si>
   <si>
     <t>10-0060</t>
@@ -128,7 +128,7 @@
     <t xml:space="preserve"> 2496810</t>
   </si>
   <si>
-    <t>Stock: 66680</t>
+    <t>Stock: 66390</t>
   </si>
   <si>
     <t>10-0058</t>
@@ -152,7 +152,7 @@
     <t xml:space="preserve"> 1828802</t>
   </si>
   <si>
-    <t>Stock: 7070</t>
+    <t>Stock: 6860</t>
   </si>
   <si>
     <t>10-0068</t>
@@ -197,7 +197,7 @@
     <t xml:space="preserve"> 1414027</t>
   </si>
   <si>
-    <t>Stock: 132725</t>
+    <t>Stock: 132555</t>
   </si>
   <si>
     <t>10-0057</t>
@@ -221,7 +221,7 @@
     <t xml:space="preserve"> 1463362</t>
   </si>
   <si>
-    <t>Stock: 46506</t>
+    <t>Stock: 46486</t>
   </si>
   <si>
     <t>10-0061</t>
@@ -347,7 +347,7 @@
     <t xml:space="preserve"> 9239359</t>
   </si>
   <si>
-    <t>Stock: 355536</t>
+    <t>Stock: 341980</t>
   </si>
   <si>
     <t>02-0098</t>
@@ -371,7 +371,7 @@
     <t xml:space="preserve"> 9239081</t>
   </si>
   <si>
-    <t>Stock: 9472</t>
+    <t>Stock: 9322</t>
   </si>
   <si>
     <t>02-0116</t>

</xml_diff>